<commit_message>
chore(Donakoko): move build files
</commit_message>
<xml_diff>
--- a/CwlExamples/Donakoko/package/LangMod/CN/Dialog/Drama/donakoko.xlsx
+++ b/CwlExamples/Donakoko/package/LangMod/CN/Dialog/Drama/donakoko.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Program Files (x86)\Steam\steamapps\common\Elin\Package\Mod_Donakoko\LangMod\CN\Dialog\Drama\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\CwlExamples\Donakoko\package\LangMod\CN\Dialog\Drama\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB41152-F9F8-4417-ACED-ACDD73604EE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4E8D30-4419-4E0C-850A-668F633B358B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1260" yWindow="4050" windowWidth="31395" windowHeight="15975" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="donakoko" sheetId="1" r:id="rId1"/>
@@ -28,12 +28,15 @@
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="155">
   <si>
     <t>step</t>
   </si>
@@ -63,9 +66,6 @@
   </si>
   <si>
     <t>text_EN</t>
-  </si>
-  <si>
-    <t>text</t>
   </si>
   <si>
     <t>*</t>
@@ -446,6 +446,111 @@
   </si>
   <si>
     <t>お姉ちゃんがここにいることを知ってくれてよかった、そうじゃないとココは退屈で死んじゃうよ！</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>text_CN</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>你好呀，來找可可有什麼事嘛？</t>
+  </si>
+  <si>
+    <t>可可等會想去拍照！</t>
+  </si>
+  <si>
+    <t>想問問可可你</t>
+  </si>
+  <si>
+    <t>有什麼想知道的嘛？可可會和你說的，畢竟可你是可可的好朋友！</t>
+  </si>
+  <si>
+    <t>姐姐是誰？</t>
+  </si>
+  <si>
+    <t>可可你會離開嗎？</t>
+  </si>
+  <si>
+    <t>暫時沒有問題了</t>
+  </si>
+  <si>
+    <t>當然是我最喜歡的小雨姐姐了！她可是一個很帥氣的人</t>
+  </si>
+  <si>
+    <t>你還沒有見過她吧，那我去聯繫一下姐姐看看</t>
+  </si>
+  <si>
+    <t>再過一段時間你就可以見到姐姐了！</t>
+  </si>
+  <si>
+    <t>說起來我也有一段時間沒見到她了，有點想她了...</t>
+  </si>
+  <si>
+    <t>娘親跟我一樣都是怪異哦，不過娘親的天賦比我強的多，我這種半吊子的不死不滅和娘親沒法比啦，還有還有，娘親的眼睛很好看！那雙瞳孔好似星河流轉！</t>
+  </si>
+  <si>
+    <t>母親的話是數位...畫筆成精哦，母親最開始的那個世界靈氣微薄不說，而其那個世界的平均壽命不超過30歲！母親能在那種世界達到現在這種程度真的很不容易。</t>
+  </si>
+  <si>
+    <t>我悄悄和你說哦，娘親們的首次相遇可是鬧出了大烏龍！我們這個種族本身就有很強的精神污染，只不過是變換成了人身隔絕了極大一部分精神污染。</t>
+  </si>
+  <si>
+    <t>而那次母親在最初路過無盡平原的時候無意中看到娘親的本體，那可是我族有史以來天賦最強的娘親啊，看到娘親的一剎那就差把母親噁心暈了（不過娘親也被母親一道劍氣斬滅了）。</t>
+  </si>
+  <si>
+    <t>要不是在之後母親看到了及時變換人身的娘親，誰知道無盡平原還會不會存在..</t>
+  </si>
+  <si>
+    <t>我上次見到她們還是兩年前，哼！把我一個人丟在這邊！</t>
+  </si>
+  <si>
+    <t>不就是不想讓可可打擾她們的二人世界嘛，真是的！</t>
+  </si>
+  <si>
+    <t>還好姐姐知道我在這邊，不然可可是會無聊死的！</t>
+  </si>
+  <si>
+    <t>現在談那些太遙遠啦，你可是我的好朋友</t>
+  </si>
+  <si>
+    <t>不是每個種族都是長生種</t>
+  </si>
+  <si>
+    <t>沒有無窮盡的壽命談何自由</t>
+  </si>
+  <si>
+    <t>至少可可會陪你們度過很久很久</t>
+  </si>
+  <si>
+    <t>直到你們睜不開眼...直到你們死去...</t>
+  </si>
+  <si>
+    <t>但是可可你依舊這般喜歡去探險，去認識各種必將死去的人</t>
+  </si>
+  <si>
+    <t>哎，每個幻想作品中長生種的悲哀，突然感覺可可好可憐</t>
+  </si>
+  <si>
+    <t>當然啦，這些都將是可可最寶貴的記憶</t>
+  </si>
+  <si>
+    <t>如果身邊都是短命種確實是這樣沒錯啦</t>
+  </si>
+  <si>
+    <t>不過不管是娘親們還是姐姐，又或者每一位長輩</t>
+  </si>
+  <si>
+    <t>她！們！都！比！可！可！厲！害！</t>
+  </si>
+  <si>
+    <t>還有玩家你一個短命種還可憐上可可了！呀呀呀！吃可可一拳！</t>
+  </si>
+  <si>
+    <t>text_ZHTW</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>text</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -597,10 +702,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="差" xfId="2" builtinId="27"/>
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="好" xfId="1" builtinId="26"/>
-    <cellStyle name="适中" xfId="3" builtinId="28"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -858,11 +963,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K66"/>
+  <dimension ref="A1:M66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K41" sqref="K41"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -878,10 +983,13 @@
     <col min="9" max="9" width="53" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="49.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="47" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="7.33203125" style="1" hidden="1"/>
+    <col min="12" max="12" width="44.33203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="49.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.33203125" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="7.33203125" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -913,592 +1021,795 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H2" s="1">
         <f>MAX(H5:H1048515)</f>
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D5" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H8" s="1">
         <v>15</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H9" s="1">
         <v>17</v>
       </c>
       <c r="I9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K9" s="1" t="s">
+      <c r="M9" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B11" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="H11" s="1">
         <v>3</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K11" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D12" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="1" t="s">
+    </row>
+    <row r="13" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="D13" s="2" t="s">
+    <row r="14" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="6" t="s">
+      <c r="D14" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="34.5" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="1" customFormat="1" ht="34.5" x14ac:dyDescent="0.3">
       <c r="H17" s="1">
         <v>7</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B19" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H19" s="1">
         <v>32</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B20" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H20" s="1">
         <v>38</v>
       </c>
       <c r="I20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K20" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J20" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="L20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B21" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H21" s="1">
         <v>47</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B22" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H22" s="1">
         <v>71</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+        <v>128</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="34.5" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" s="1" customFormat="1" ht="34.5" x14ac:dyDescent="0.3">
       <c r="H25" s="1">
         <v>33</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+        <v>129</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H26" s="1">
         <v>34</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H27" s="1">
         <v>35</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="34.5" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" s="1" customFormat="1" ht="34.5" x14ac:dyDescent="0.3">
       <c r="H28" s="1">
         <v>36</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+        <v>132</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B30" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="69" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" s="1" customFormat="1" ht="69" x14ac:dyDescent="0.3">
       <c r="H33" s="1">
         <v>39</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="86.25" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" s="1" customFormat="1" ht="86.25" x14ac:dyDescent="0.3">
       <c r="H34" s="1">
         <v>40</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="69" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+      <c r="L34" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M34" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" s="1" customFormat="1" ht="69" x14ac:dyDescent="0.3">
       <c r="H35" s="1">
         <v>41</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="86.25" x14ac:dyDescent="0.3">
+        <v>135</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M35" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" s="1" customFormat="1" ht="86.25" x14ac:dyDescent="0.3">
       <c r="H36" s="1">
         <v>42</v>
       </c>
       <c r="I36" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" s="1" customFormat="1" ht="69" x14ac:dyDescent="0.3">
+      <c r="I37" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="J36" s="1" t="s">
+      <c r="J37" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K36" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="69" x14ac:dyDescent="0.3">
-      <c r="I37" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="J37" s="1" t="s">
+      <c r="K37" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="L37" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="K37" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="M37" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="34.5" x14ac:dyDescent="0.3">
       <c r="H38" s="1">
         <v>43</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="51.75" x14ac:dyDescent="0.3">
+        <v>138</v>
+      </c>
+      <c r="L38" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M38" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="51.75" x14ac:dyDescent="0.3">
       <c r="H39" s="1">
         <v>44</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K39" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="34.5" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+      <c r="L39" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" ht="34.5" x14ac:dyDescent="0.3">
       <c r="H40" s="1">
         <v>45</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B42" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" ht="34.5" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" ht="34.5" x14ac:dyDescent="0.3">
       <c r="H45" s="1">
         <v>48</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="M45" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H46" s="1">
         <v>49</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="J46" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K46" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" ht="34.5" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M46" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="34.5" x14ac:dyDescent="0.3">
       <c r="H47" s="1">
         <v>50</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K47" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+        <v>143</v>
+      </c>
+      <c r="L47" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H48" s="1">
         <v>51</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J48" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+        <v>144</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H49" s="1">
         <v>52</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" ht="34.5" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+      <c r="L49" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="M49" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" ht="34.5" x14ac:dyDescent="0.3">
       <c r="B51" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H51" s="1">
         <v>54</v>
       </c>
       <c r="I51" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="J51" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="J51" s="1" t="s">
-        <v>108</v>
-      </c>
       <c r="K51" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="34.5" x14ac:dyDescent="0.3">
+        <v>146</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M51" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" ht="34.5" x14ac:dyDescent="0.3">
       <c r="B52" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H52" s="1">
         <v>55</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M52" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" ht="51.75" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" ht="51.75" x14ac:dyDescent="0.3">
       <c r="H55" s="1">
         <v>84</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K55" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M55" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B57" s="5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" ht="34.5" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" ht="34.5" x14ac:dyDescent="0.3">
       <c r="H60" s="1">
         <v>81</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K60" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" ht="34.5" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" ht="34.5" x14ac:dyDescent="0.3">
       <c r="H61" s="1">
         <v>82</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M61" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="H62" s="1">
         <v>83</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" ht="34.5" x14ac:dyDescent="0.3">
+        <v>151</v>
+      </c>
+      <c r="L62" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M62" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" ht="34.5" x14ac:dyDescent="0.3">
       <c r="H63" s="1">
         <v>57</v>
       </c>
       <c r="I63" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J63" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>46</v>
+        <v>152</v>
+      </c>
+      <c r="L63" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M63" s="1" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B65" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="66" spans="2:2" s="3" customFormat="1" x14ac:dyDescent="0.3"/>

</xml_diff>